<commit_message>
completes travis test case
</commit_message>
<xml_diff>
--- a/data/Travis150/Travis150_Gas_Data.xlsx
+++ b/data/Travis150/Travis150_Gas_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youse\Desktop\Research\Austin Case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaarthiksundar/Documents/codes/texas-gas-grid/data/Travis150/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACBF027-1157-42C6-8DB9-1E92C2199913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C19EE84-1AE5-1C4A-AB79-E9BC5FD18CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="3945" windowWidth="19050" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12240" yWindow="3940" windowWidth="19060" windowHeight="15440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="4" r:id="rId1"/>
@@ -289,12 +289,6 @@
     <t>Capacity (MMCF/mo)</t>
   </si>
   <si>
-    <t>Sarting Node</t>
-  </si>
-  <si>
-    <t>Ending Ndoe</t>
-  </si>
-  <si>
     <t>Diameter (mm)</t>
   </si>
   <si>
@@ -311,6 +305,12 @@
   </si>
   <si>
     <t xml:space="preserve"> MW Consumption</t>
+  </si>
+  <si>
+    <t>Starting Node</t>
+  </si>
+  <si>
+    <t>Ending Node</t>
   </si>
 </sst>
 </file>
@@ -635,9 +635,9 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -654,10 +654,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
@@ -677,7 +677,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -697,7 +697,7 @@
         <v>1399.6191841331499</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -717,7 +717,7 @@
         <v>1399.75836974514</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -737,7 +737,7 @@
         <v>1404.86104963856</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -757,7 +757,7 @@
         <v>1386.12310222306</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -777,7 +777,7 @@
         <v>1421.39127916648</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1414.7185632465701</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -817,7 +817,7 @@
         <v>1415.11121462083</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -837,7 +837,7 @@
         <v>1443.23473661656</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -857,7 +857,7 @@
         <v>1389.9085817817499</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -877,7 +877,7 @@
         <v>1377.6265077707201</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1470.90654404917</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -917,7 +917,7 @@
         <v>1442.59474501163</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -937,7 +937,7 @@
         <v>1377.7644421725699</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -957,7 +957,7 @@
         <v>1399.2995302192001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -977,7 +977,7 @@
         <v>1662.25502022869</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -997,7 +997,7 @@
         <v>1379.45759455286</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>1761.56776699032</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>1384.33946948429</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>1399.8951662571601</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>1413.4256663507599</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>1381.46706282741</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>1381.2252117067401</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>1537.4620296518699</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>1761.8972180834501</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>1662.33704937371</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>1537.5585245105499</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>1521.42194227698</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>1443.84342885764</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>1424.8090789575199</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>1423.3909881248101</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>1405.1911640942999</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>1400.0669349820701</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>1399.9822579275501</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>1399.75848474958</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>1399.73571893041</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>1399.68832618492</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>1471.2206780080901</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>1442.59787660288</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>1415.99130600834</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>1413.5476577229299</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>1384.6444792688701</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>1381.9148639099899</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>1381.50315611923</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>1379.74193301746</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>1378.3467076043401</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1610,12 +1610,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1629,10 +1629,10 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>101.4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>693.75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>772.85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>617.01</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>487.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1764,9 +1764,9 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>15</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>17</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>19</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>21</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>22</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>23</v>
       </c>
@@ -1966,9 +1966,9 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
@@ -2000,32 +2000,38 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>24</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>683093.48986871296</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>25</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>669354.71945425298</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>26</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>656360.83871903503</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>27</v>
       </c>
@@ -2105,7 +2111,7 @@
         <v>629699.37290829106</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>28</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>464770.021800805</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>29</v>
       </c>
@@ -2145,7 +2151,7 @@
         <v>444321.344935678</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>30</v>
       </c>
@@ -2165,7 +2171,7 @@
         <v>312022.80259117699</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>31</v>
       </c>
@@ -2185,7 +2191,7 @@
         <v>237504.731268659</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>32</v>
       </c>
@@ -2205,7 +2211,7 @@
         <v>153718.80076379899</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>33</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>46300.517600004699</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>34</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>30727.053229014102</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>35</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>30366.013775188901</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>36</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>12246.3953474835</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>25</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>13738.7704144607</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>26</v>
       </c>
@@ -2325,7 +2331,7 @@
         <v>12993.880735217899</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>27</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>26661.465810743499</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>28</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>164929.351107486</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>38</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>143344.855132722</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>39</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>126025.186867414</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>40</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>67191.880749690899</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>29</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>20448.676865126599</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>30</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>132298.54234449999</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>41</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>113935.47792342</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>42</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>99243.767861227403</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>43</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>73243.814426664598</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>44</v>
       </c>
@@ -2545,7 +2551,7 @@
         <v>60664.067182599101</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>45</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>45090.996100773897</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>46</v>
       </c>
@@ -2585,7 +2591,7 @@
         <v>19872.901527000198</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>31</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>74518.071322518197</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>32</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>83785.930504860502</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>33</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>107418.283163794</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>47</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>14078.9655425203</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2685,7 +2691,7 @@
         <v>15573.464370990599</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>361.03945382517702</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2725,7 +2731,7 @@
         <v>18119.618427705402</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -2745,7 +2751,7 @@
         <v>12246.3953474835</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>21584.495974763999</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2785,7 +2791,7 @@
         <v>17319.668265308399</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2805,7 +2811,7 @@
         <v>58833.306117722997</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2825,7 +2831,7 @@
         <v>18363.0644210799</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>14691.7100621931</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2865,7 +2871,7 @@
         <v>25999.953434562802</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2885,7 +2891,7 @@
         <v>12579.7472440655</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>15573.071081825199</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>25218.0945737736</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>47</v>
       </c>

</xml_diff>